<commit_message>
Utah water rights update.
Utah water rights update.  Changes to water source type.
</commit_message>
<xml_diff>
--- a/Utah/WaterAllocation/UT_Allocation Schema Mapping_WaDEQA.xlsx
+++ b/Utah/WaterAllocation/UT_Allocation Schema Mapping_WaDEQA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Utah\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAE3B0A-666F-47C3-B409-C6D41BB01F69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A20C57-15AA-4645-85B6-B1B7C6BBE42F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="8" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Methods" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="AllocationsAmounts_fact" sheetId="7" r:id="rId6"/>
     <sheet name="strLiteralToDateString" sheetId="10" r:id="rId7"/>
     <sheet name="BeneficialUseCategory" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="355">
   <si>
     <t>AllocationAmount</t>
   </si>
@@ -1657,6 +1658,261 @@
   </si>
   <si>
     <t>concantate with a counter and 'UT'</t>
+  </si>
+  <si>
+    <t>DIS</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>DIO</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>IO</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>OX</t>
+  </si>
+  <si>
+    <t>IOS</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>IX</t>
+  </si>
+  <si>
+    <t>DIOS</t>
+  </si>
+  <si>
+    <t>DX</t>
+  </si>
+  <si>
+    <t>DOS</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>IMS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>DSX</t>
+  </si>
+  <si>
+    <t>DIMOS</t>
+  </si>
+  <si>
+    <t>SX</t>
+  </si>
+  <si>
+    <t>DIMS</t>
+  </si>
+  <si>
+    <t>IMO</t>
+  </si>
+  <si>
+    <t>DIOP</t>
+  </si>
+  <si>
+    <t>IMOSX</t>
+  </si>
+  <si>
+    <t>DOX</t>
+  </si>
+  <si>
+    <t>PX</t>
+  </si>
+  <si>
+    <t>DIX</t>
+  </si>
+  <si>
+    <t>DISX</t>
+  </si>
+  <si>
+    <t>DMO</t>
+  </si>
+  <si>
+    <t>ISX</t>
+  </si>
+  <si>
+    <t>OSX</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>DMS</t>
+  </si>
+  <si>
+    <t>DISP</t>
+  </si>
+  <si>
+    <t>IOP</t>
+  </si>
+  <si>
+    <t>ISP</t>
+  </si>
+  <si>
+    <t>DIOSP</t>
+  </si>
+  <si>
+    <t>OPX</t>
+  </si>
+  <si>
+    <t>DOSX</t>
+  </si>
+  <si>
+    <t>DIOSPX</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>DIMO</t>
+  </si>
+  <si>
+    <t>DIM</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>IMP</t>
+  </si>
+  <si>
+    <t>IMOS</t>
+  </si>
+  <si>
+    <t>OSP</t>
+  </si>
+  <si>
+    <t>DIP</t>
+  </si>
+  <si>
+    <t>DIMOP</t>
+  </si>
+  <si>
+    <t>MOX</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>IMX</t>
+  </si>
+  <si>
+    <t>DMX</t>
+  </si>
+  <si>
+    <t>DIMOSP</t>
+  </si>
+  <si>
+    <t>MSP</t>
+  </si>
+  <si>
+    <t>DSP</t>
+  </si>
+  <si>
+    <t>DOP</t>
+  </si>
+  <si>
+    <t>DMOSX</t>
+  </si>
+  <si>
+    <t>DIOX</t>
+  </si>
+  <si>
+    <t>DISPX</t>
+  </si>
+  <si>
+    <t>MOS</t>
+  </si>
+  <si>
+    <t>IOX</t>
+  </si>
+  <si>
+    <t>DPX</t>
+  </si>
+  <si>
+    <t>IMSP</t>
+  </si>
+  <si>
+    <t>MOP</t>
+  </si>
+  <si>
+    <t>IOSX</t>
+  </si>
+  <si>
+    <t>DIMOSPX</t>
+  </si>
+  <si>
+    <t>DIMOSX</t>
+  </si>
+  <si>
+    <t>IOSP</t>
+  </si>
+  <si>
+    <t>MSX</t>
+  </si>
+  <si>
+    <t>IOSPX</t>
+  </si>
+  <si>
+    <t>IPX</t>
+  </si>
+  <si>
+    <t>DIOSX</t>
+  </si>
+  <si>
+    <t>IMOP</t>
+  </si>
+  <si>
+    <t>DOPX</t>
+  </si>
+  <si>
+    <t>DMOP</t>
+  </si>
+  <si>
+    <t>DIMOX</t>
+  </si>
+  <si>
+    <t>DIMX</t>
+  </si>
+  <si>
+    <t>DMOS</t>
+  </si>
+  <si>
+    <t>IMOSP</t>
+  </si>
+  <si>
+    <t>DIMSP</t>
   </si>
 </sst>
 </file>
@@ -5286,7 +5542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
@@ -7012,4 +7268,487 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9330F944-A4DF-4853-937F-B846AC9F3E61}">
+  <dimension ref="A1:A93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A317488"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A317487">
+    <sortCondition ref="A2:A317487"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>